<commit_message>
Adding #115, #182, #183, #189, #180
New checks for forced grants, backup compression default off, Adam
Machanic's make_parallel function, NUMA nodes, fixing named instance
check.
</commit_message>
<xml_diff>
--- a/sp_Blitz/sp_Blitz™-CheckID-List.xlsx
+++ b/sp_Blitz/sp_Blitz™-CheckID-List.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="900" windowWidth="26260" windowHeight="23420" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="30360" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="291">
   <si>
     <t>Backups Not Performed Recently</t>
   </si>
@@ -911,6 +911,24 @@
   </si>
   <si>
     <t>sp_Blitz™ Check ID List - v24 June 23, 2013</t>
+  </si>
+  <si>
+    <t>Hardware - NUMA Config</t>
+  </si>
+  <si>
+    <t>Parallelism Rocket Surgery</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/makeparallel</t>
+  </si>
+  <si>
+    <t>Backup Compression Default Off</t>
+  </si>
+  <si>
+    <t>Memory Pressure Affecting Queries</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/grants</t>
   </si>
 </sst>
 </file>
@@ -1976,13 +1994,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E178"/>
+  <dimension ref="A1:E182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B96" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="E183" sqref="E183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4966,6 +4984,71 @@
       </c>
       <c r="E178" s="6" t="s">
         <v>282</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5">
+      <c r="A179" s="4">
+        <v>114</v>
+      </c>
+      <c r="B179" s="5">
+        <v>250</v>
+      </c>
+      <c r="C179" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D179" s="5" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
+      <c r="A180" s="4">
+        <v>115</v>
+      </c>
+      <c r="B180" s="5">
+        <v>110</v>
+      </c>
+      <c r="C180" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D180" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="E180" s="6" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
+      <c r="A181" s="4">
+        <v>116</v>
+      </c>
+      <c r="B181" s="5">
+        <v>200</v>
+      </c>
+      <c r="C181" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D181" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="E181" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5">
+      <c r="A182" s="4">
+        <v>117</v>
+      </c>
+      <c r="B182" s="5">
+        <v>100</v>
+      </c>
+      <c r="C182" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D182" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="E182" s="6" t="s">
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -4997,10 +5080,13 @@
     <hyperlink ref="E176" r:id="rId22"/>
     <hyperlink ref="E177" r:id="rId23"/>
     <hyperlink ref="E178" r:id="rId24"/>
+    <hyperlink ref="E180" r:id="rId25"/>
+    <hyperlink ref="E181" r:id="rId26"/>
+    <hyperlink ref="E182" r:id="rId27"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId25"/>
+  <legacyDrawing r:id="rId28"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Adding check 118 for key lookups in plan cache
</commit_message>
<xml_diff>
--- a/sp_Blitz/sp_Blitz™-CheckID-List.xlsx
+++ b/sp_Blitz/sp_Blitz™-CheckID-List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="30360" activeTab="1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="293">
   <si>
     <t>Backups Not Performed Recently</t>
   </si>
@@ -929,6 +929,12 @@
   </si>
   <si>
     <t>http://BrentOzar.com/go/grants</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/lookup</t>
+  </si>
+  <si>
+    <t>RID or Key Lookups</t>
   </si>
 </sst>
 </file>
@@ -1994,13 +2000,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E182"/>
+  <dimension ref="A1:E183"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B96" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B97" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E183" sqref="E183"/>
+      <selection pane="bottomRight" activeCell="B184" sqref="B184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5049,6 +5055,23 @@
       </c>
       <c r="E182" s="6" t="s">
         <v>290</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5">
+      <c r="A183" s="4">
+        <v>118</v>
+      </c>
+      <c r="B183" s="5">
+        <v>120</v>
+      </c>
+      <c r="C183" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D183" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="E183" s="6" t="s">
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -5083,10 +5106,11 @@
     <hyperlink ref="E180" r:id="rId25"/>
     <hyperlink ref="E181" r:id="rId26"/>
     <hyperlink ref="E182" r:id="rId27"/>
+    <hyperlink ref="E183" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId28"/>
+  <legacyDrawing r:id="rId29"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added check 119 for TDE certificates that have not been backed up recently
:lock:
</commit_message>
<xml_diff>
--- a/sp_Blitz/sp_Blitz™-CheckID-List.xlsx
+++ b/sp_Blitz/sp_Blitz™-CheckID-List.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="294">
   <si>
     <t>Backups Not Performed Recently</t>
   </si>
@@ -935,6 +935,9 @@
   </si>
   <si>
     <t>RID or Key Lookups</t>
+  </si>
+  <si>
+    <t>TDE Certificate Not Backed Up Recently</t>
   </si>
 </sst>
 </file>
@@ -2000,13 +2003,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E183"/>
+  <dimension ref="A1:E184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B97" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B100" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B184" sqref="B184"/>
+      <selection pane="bottomRight" activeCell="A185" sqref="A185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5072,6 +5075,23 @@
       </c>
       <c r="E183" s="6" t="s">
         <v>291</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5">
+      <c r="A184" s="4">
+        <v>119</v>
+      </c>
+      <c r="B184" s="5">
+        <v>1</v>
+      </c>
+      <c r="C184" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D184" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="E184" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -5107,10 +5127,11 @@
     <hyperlink ref="E181" r:id="rId26"/>
     <hyperlink ref="E182" r:id="rId27"/>
     <hyperlink ref="E183" r:id="rId28"/>
+    <hyperlink ref="E184" r:id="rId29"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId29"/>
+  <legacyDrawing r:id="rId30"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Closing #219 adding check 120 for backups without WITH CHECKSUM parameter
:neckbeard:
</commit_message>
<xml_diff>
--- a/sp_Blitz/sp_Blitz™-CheckID-List.xlsx
+++ b/sp_Blitz/sp_Blitz™-CheckID-List.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="295">
   <si>
     <t>Backups Not Performed Recently</t>
   </si>
@@ -938,6 +938,9 @@
   </si>
   <si>
     <t>TDE Certificate Not Backed Up Recently</t>
+  </si>
+  <si>
+    <t>Backup Checksums Not Used</t>
   </si>
 </sst>
 </file>
@@ -1024,7 +1027,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1032,6 +1035,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -1055,13 +1059,14 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="10">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="6" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2003,10 +2008,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E184"/>
+  <dimension ref="A1:E185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B100" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B181" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A185" sqref="A185"/>
@@ -5092,6 +5097,23 @@
       </c>
       <c r="E184" s="6" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5">
+      <c r="A185" s="4">
+        <v>120</v>
+      </c>
+      <c r="B185" s="5">
+        <v>50</v>
+      </c>
+      <c r="C185" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D185" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="E185" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v34 work in progress
Added #240, #262, #263.
</commit_message>
<xml_diff>
--- a/sp_Blitz/sp_Blitz™-CheckID-List.xlsx
+++ b/sp_Blitz/sp_Blitz™-CheckID-List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23380" windowHeight="28340" activeTab="1"/>
+    <workbookView xWindow="1160" yWindow="0" windowWidth="26000" windowHeight="28340" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="303">
   <si>
     <t>Backups Not Performed Recently</t>
   </si>
@@ -958,7 +958,13 @@
     <t>http://BrentOzar.com/go/busyagent</t>
   </si>
   <si>
-    <t>sp_Blitz™ Check ID List - v32 January 19, 2014</t>
+    <t>sp_Blitz™ Check ID List - v34 April 2, 2014</t>
+  </si>
+  <si>
+    <t>Deadlocks Happening Daily</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/deadlocks</t>
   </si>
 </sst>
 </file>
@@ -2042,13 +2048,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E188"/>
+  <dimension ref="A1:E189"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B139" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A190" sqref="A190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5199,6 +5205,23 @@
       </c>
       <c r="E188" s="6" t="s">
         <v>299</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5">
+      <c r="A189" s="4">
+        <v>124</v>
+      </c>
+      <c r="B189" s="5">
+        <v>100</v>
+      </c>
+      <c r="C189" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D189" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="E189" s="6" t="s">
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -5238,10 +5261,11 @@
     <hyperlink ref="E186" r:id="rId30"/>
     <hyperlink ref="E187" r:id="rId31"/>
     <hyperlink ref="E188" r:id="rId32"/>
+    <hyperlink ref="E189" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId33"/>
+  <legacyDrawing r:id="rId34"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>